<commit_message>
export hourly with  params
</commit_message>
<xml_diff>
--- a/inst/application/www/Output_Selection_template.xlsx
+++ b/inst/application/www/Output_Selection_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Datastorm\Documents\git\antaresVizMedTSO\inst\application\www\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenoitThieurmel\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC9B452-FF9C-44AB-8064-BED359CC7779}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21F68D5-F414-485D-9D82-20473F47E4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{D77C83E6-B695-4B37-B3DE-F053925C20A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D77C83E6-B695-4B37-B3DE-F053925C20A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual_Selection" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="287">
   <si>
     <t>Links</t>
   </si>
@@ -518,135 +518,9 @@
     <t>Areas_Districts</t>
   </si>
   <si>
-    <t>nuclear_nuclear</t>
-  </si>
-  <si>
-    <t>lignite_old 1</t>
-  </si>
-  <si>
-    <t>lignite_old 2</t>
-  </si>
-  <si>
-    <t>lignite_new</t>
-  </si>
-  <si>
-    <t>lignite_ccs</t>
-  </si>
-  <si>
-    <t>hard coal_old 1</t>
-  </si>
-  <si>
-    <t>hard coal_old 2</t>
-  </si>
-  <si>
-    <t>hard coal_new</t>
-  </si>
-  <si>
-    <t>hard coal_ccs</t>
-  </si>
-  <si>
-    <t>gas_conventional old 1</t>
-  </si>
-  <si>
-    <t>gas_conventional old 2</t>
-  </si>
-  <si>
-    <t>gas_ccgt old 1</t>
-  </si>
-  <si>
-    <t>gas_ccgt old 2</t>
-  </si>
-  <si>
-    <t>gas_ccgt present 1</t>
-  </si>
-  <si>
-    <t>gas_ccgt present 2</t>
-  </si>
-  <si>
-    <t>gas_ccgt new</t>
-  </si>
-  <si>
-    <t>gas_ccgt ccs</t>
-  </si>
-  <si>
-    <t>gas_ocgt old</t>
-  </si>
-  <si>
-    <t>gas_ocgt new</t>
-  </si>
-  <si>
-    <t>light oil_light oil</t>
-  </si>
-  <si>
-    <t>heavy oil_old 1</t>
-  </si>
-  <si>
-    <t>heavy oil_old 2</t>
-  </si>
-  <si>
-    <t>oil shale_old</t>
-  </si>
-  <si>
-    <t>oil shale_new</t>
-  </si>
-  <si>
-    <t>H. ROR</t>
-  </si>
-  <si>
-    <t>H. STOR</t>
-  </si>
-  <si>
-    <t>WIND</t>
-  </si>
-  <si>
-    <t>SOLAR</t>
-  </si>
-  <si>
-    <t>MISC. NDG</t>
-  </si>
-  <si>
-    <t>lignite_bio</t>
-  </si>
-  <si>
-    <t>hard coal_bio</t>
-  </si>
-  <si>
-    <t>gas_bio</t>
-  </si>
-  <si>
-    <t>light oil_bio</t>
-  </si>
-  <si>
-    <t>heavy oil_bio</t>
-  </si>
-  <si>
-    <t>oil shale_bio</t>
-  </si>
-  <si>
-    <t>LOAD</t>
-  </si>
-  <si>
-    <t>BALANCE</t>
-  </si>
-  <si>
-    <t>SPIL. ENRG</t>
-  </si>
-  <si>
-    <t>UNSP. ENRG</t>
-  </si>
-  <si>
-    <t>MRG. PRICE</t>
-  </si>
-  <si>
     <t>Market_Data_Code</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>Nuclear [MW]</t>
   </si>
   <si>
@@ -737,75 +611,36 @@
     <t>Oil shale biofuel [MW]</t>
   </si>
   <si>
-    <t>OV. COST</t>
-  </si>
-  <si>
     <t>Overall cost [€]</t>
   </si>
   <si>
-    <t>(= operating cost + unsupplied energy cost + spilled energy cost)</t>
-  </si>
-  <si>
-    <t>OP. COST</t>
-  </si>
-  <si>
     <t>Operating Cost [€]</t>
   </si>
   <si>
-    <t>(= Proportional cost + Non-Proportional cost)</t>
-  </si>
-  <si>
-    <t>NP COST</t>
-  </si>
-  <si>
     <t>Non Proportional costs [€]</t>
   </si>
   <si>
-    <t>Non Proportional costs of the dispatchable Thermal plants (start-up and fixed cost)</t>
-  </si>
-  <si>
     <t>Marginal Price [€/MWh]</t>
   </si>
   <si>
-    <t>incl. unsupplied energy cost and spilled energy cost</t>
-  </si>
-  <si>
-    <t>CO2 EMIS.</t>
-  </si>
-  <si>
     <t>CO2 emissions [tCO2]</t>
   </si>
   <si>
     <t>Balance [MW]</t>
   </si>
   <si>
-    <t>ROW BAL.</t>
-  </si>
-  <si>
     <t>RoW Balance [MW]</t>
   </si>
   <si>
-    <t>Balance with areas outside the modeled system</t>
-  </si>
-  <si>
     <t>Pump Storage (turbine) [MW]</t>
   </si>
   <si>
-    <t>if value is positive ; doit inclure la suppresion du nœud virtuel Turbine</t>
-  </si>
-  <si>
     <t>Pump Storage (pump) [MW]</t>
   </si>
   <si>
-    <t>if value is negative ; doit inclure la suppresion du nœud virtuel Turbine</t>
-  </si>
-  <si>
     <t>Others renewable [MW]</t>
   </si>
   <si>
-    <t>eq. Misc. Gen (CHP+BioMass+Biogas+Waste+Geothermal+other)</t>
-  </si>
-  <si>
     <t>Demand [MW]</t>
   </si>
   <si>
@@ -815,54 +650,27 @@
     <t>Wind generation [MW]</t>
   </si>
   <si>
-    <t>incl. Onshore and Offshore</t>
-  </si>
-  <si>
     <t>Solar generation [MW]</t>
   </si>
   <si>
-    <t>incl. PV and Thermal</t>
-  </si>
-  <si>
-    <t>NUCLEAR</t>
-  </si>
-  <si>
     <t>Nuclear generation [MW]</t>
   </si>
   <si>
-    <t>COAL</t>
-  </si>
-  <si>
     <t>Coal generation [MW]</t>
   </si>
   <si>
-    <t>LIGNITE</t>
-  </si>
-  <si>
     <t>Lignite generation [MW]</t>
   </si>
   <si>
-    <t>GAS</t>
-  </si>
-  <si>
     <t>Gas generation [MW]</t>
   </si>
   <si>
-    <t>OIL</t>
-  </si>
-  <si>
     <t>Oil generation [MW]</t>
   </si>
   <si>
-    <t>MIX. FUEL</t>
-  </si>
-  <si>
     <t>Mix Fuel generation [MW]</t>
   </si>
   <si>
-    <t>MISC. DTG</t>
-  </si>
-  <si>
     <t>Other Fuel generation [MW]</t>
   </si>
   <si>
@@ -875,56 +683,224 @@
     <t>Dumped Energy [MW]</t>
   </si>
   <si>
-    <t>LOLD</t>
-  </si>
-  <si>
     <t>Loss of Load Duration [h]</t>
   </si>
   <si>
-    <t>LOLP</t>
-  </si>
-  <si>
     <t>Loss of Load Probability [%]</t>
   </si>
   <si>
-    <t>AVL DTG</t>
-  </si>
-  <si>
     <t>Available Thermal Generation [MW]</t>
   </si>
   <si>
-    <t>DTG MRG</t>
-  </si>
-  <si>
     <t>Margin on Thermal Units [MW]</t>
   </si>
   <si>
-    <t>MAX MRG</t>
-  </si>
-  <si>
     <t>Maximum Margin [MW]</t>
   </si>
   <si>
     <t>NODU</t>
   </si>
   <si>
-    <t>Cluster</t>
-  </si>
-  <si>
-    <t>ANTARES_naming</t>
-  </si>
-  <si>
-    <t>PSP_TURB</t>
-  </si>
-  <si>
-    <t>PSP_PUMP</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>cluster - nuclear_nuclear</t>
+  </si>
+  <si>
+    <t>cluster - hard coal_old 1</t>
+  </si>
+  <si>
+    <t>cluster - hard coal_old 2</t>
+  </si>
+  <si>
+    <t>cluster - hard coal_new</t>
+  </si>
+  <si>
+    <t>cluster - hard coal_ccs</t>
+  </si>
+  <si>
+    <t>cluster - lignite_old 1</t>
+  </si>
+  <si>
+    <t>cluster - lignite_old 2</t>
+  </si>
+  <si>
+    <t>cluster - lignite_new</t>
+  </si>
+  <si>
+    <t>cluster - lignite_ccs</t>
+  </si>
+  <si>
+    <t>cluster - gas_conventional old 1</t>
+  </si>
+  <si>
+    <t>cluster - gas_conventional old 2</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt old 1</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt old 2</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt present 1</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt present 2</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt new</t>
+  </si>
+  <si>
+    <t>cluster - gas_ccgt ccs</t>
+  </si>
+  <si>
+    <t>cluster - gas_ocgt old</t>
+  </si>
+  <si>
+    <t>cluster - gas_ocgt new</t>
+  </si>
+  <si>
+    <t>cluster - light oil_light oil</t>
+  </si>
+  <si>
+    <t>cluster - heavy oil_old 1</t>
+  </si>
+  <si>
+    <t>cluster - heavy oil_old 2</t>
+  </si>
+  <si>
+    <t>cluster - oil shale_old</t>
+  </si>
+  <si>
+    <t>cluster - oil shale_new</t>
+  </si>
+  <si>
+    <t>cluster - lignite_bio</t>
+  </si>
+  <si>
+    <t>cluster - hard coal_bio</t>
+  </si>
+  <si>
+    <t>cluster - gas_bio</t>
+  </si>
+  <si>
+    <t>cluster - light oil_bio</t>
+  </si>
+  <si>
+    <t>cluster - heavy oil_bio</t>
+  </si>
+  <si>
+    <t>cluster - oil shale_bio</t>
+  </si>
+  <si>
+    <t>production</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>`OV. COST`</t>
+  </si>
+  <si>
+    <t>`OP. COST`</t>
+  </si>
+  <si>
+    <t>`NP COST`</t>
+  </si>
+  <si>
+    <t>`MRG. PRICE`</t>
+  </si>
+  <si>
+    <t>`CO2 EMIS.`</t>
+  </si>
+  <si>
+    <t>`BALANCE`</t>
+  </si>
+  <si>
+    <t>`ROW BAL.`</t>
+  </si>
+  <si>
+    <t>ifelse(`PSP` &gt; 0, `PSP`, 0)</t>
+  </si>
+  <si>
+    <t>ifelse(`PSP` &lt; 0, `PSP`, 0)</t>
+  </si>
+  <si>
+    <t>`MISC. NDG`</t>
+  </si>
+  <si>
+    <t>`LOAD`</t>
+  </si>
+  <si>
+    <t>`H. ROR`</t>
+  </si>
+  <si>
+    <t>`WIND`</t>
+  </si>
+  <si>
+    <t>`SOLAR`</t>
+  </si>
+  <si>
+    <t>`NUCLEAR`</t>
+  </si>
+  <si>
+    <t>`COAL`</t>
+  </si>
+  <si>
+    <t>`LIGNITE`</t>
+  </si>
+  <si>
+    <t>`GAS`</t>
+  </si>
+  <si>
+    <t>`OIL`</t>
+  </si>
+  <si>
+    <t>`MIX. FUEL`</t>
+  </si>
+  <si>
+    <t>`MISC. DTG`</t>
+  </si>
+  <si>
+    <t>`H. STOR`</t>
+  </si>
+  <si>
+    <t>`UNSP. ENRG`</t>
+  </si>
+  <si>
+    <t>`SPIL. ENRG`</t>
+  </si>
+  <si>
+    <t>`LOLD`</t>
+  </si>
+  <si>
+    <t>`LOLP`</t>
+  </si>
+  <si>
+    <t>`AVL DTG`</t>
+  </si>
+  <si>
+    <t>`DTG MRG`</t>
+  </si>
+  <si>
+    <t>`MAX MRG`</t>
+  </si>
+  <si>
+    <t>`NODU`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -969,6 +945,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -984,7 +973,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1103,49 +1092,113 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1464,15 +1517,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6269D062-6DED-4CF7-AAB6-D21CF22BAB73}">
   <dimension ref="A1:B119"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
@@ -1480,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1504,7 +1557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1512,7 +1565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1520,7 +1573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1528,7 +1581,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1589,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1544,7 +1597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1552,7 +1605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1560,7 +1613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1568,7 +1621,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1576,7 +1629,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1584,7 +1637,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1592,7 +1645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -1600,7 +1653,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -1608,7 +1661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -1616,7 +1669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -1624,7 +1677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -1632,7 +1685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1640,7 +1693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -1648,7 +1701,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -1656,7 +1709,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -1664,7 +1717,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
@@ -1672,7 +1725,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
@@ -1680,7 +1733,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -1688,7 +1741,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
@@ -1696,7 +1749,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
@@ -1704,7 +1757,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
@@ -1712,7 +1765,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
@@ -1720,7 +1773,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>61</v>
       </c>
@@ -1728,7 +1781,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -1736,7 +1789,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -1744,7 +1797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
@@ -1752,7 +1805,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>69</v>
       </c>
@@ -1760,7 +1813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
@@ -1768,7 +1821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>73</v>
       </c>
@@ -1776,7 +1829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
@@ -1784,7 +1837,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>77</v>
       </c>
@@ -1792,7 +1845,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>79</v>
       </c>
@@ -1800,7 +1853,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>81</v>
       </c>
@@ -1808,463 +1861,463 @@
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2" t="s">
         <v>159</v>
@@ -2277,940 +2330,887 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA0C1F2-E3A3-48EB-881E-BF01D90AA1B6}">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="B20" s="2"/>
+      <c r="C20" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="2"/>
+      <c r="C21" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="B30" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="B31" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
-      <c r="B32" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="2"/>
+      <c r="C33" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
-      <c r="B35" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
-      <c r="B36" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="B36" s="2"/>
+      <c r="C36" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
-      <c r="B37" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
-      <c r="B39" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="2"/>
+      <c r="C39" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
-      <c r="B40" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="B40" s="2"/>
+      <c r="C40" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
-      <c r="B41" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="2"/>
+      <c r="C41" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
-      <c r="B42" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
-      <c r="B43" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="8" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="8" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
-      <c r="C69" s="2" t="s">
+      <c r="C69" s="8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="8" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="8" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="8" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
-      <c r="C75" s="2" t="s">
+      <c r="C75" s="8" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
-      <c r="C85" s="2" t="s">
+      <c r="C85" s="8" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="8" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="8" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
-      <c r="C90" s="2" t="s">
+      <c r="C90" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="8" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
-      <c r="C95" s="2" t="s">
+      <c r="C95" s="8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
-      <c r="C96" s="2" t="s">
+      <c r="C96" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="8" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="8" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="8" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="8" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="8" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
-      <c r="C108" s="2" t="s">
+      <c r="C108" s="8" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
-      <c r="C110" s="2" t="s">
+      <c r="C110" s="8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
-      <c r="C114" s="2" t="s">
+      <c r="C114" s="8" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="8" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="8" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3223,649 +3223,690 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B57E84-B55D-4563-ABB5-693AD42469D5}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="37.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="68.5546875" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B42" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="16" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="B43" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="B44" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="10" t="s">
+      <c r="B45" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="16" t="s">
         <v>206</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B5" s="10" t="s">
+      <c r="B46" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" s="10" t="s">
+      <c r="B47" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="B48" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="B49" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B9" s="8" t="s">
+      <c r="B50" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="B51" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="B52" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="B12" s="10" t="s">
+      <c r="B53" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="B54" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="B55" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="B56" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="10" t="s">
+      <c r="B57" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="18" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="B58" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="B59" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="B60" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>246</v>
-      </c>
-      <c r="C36" s="7"/>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13" t="s">
-        <v>293</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C41" s="7" t="s">
+      <c r="B61" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C61" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
-        <v>265</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="C48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="C55" s="7"/>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C56" s="7"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="B57" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="B58" s="12" t="s">
-        <v>285</v>
-      </c>
-      <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="C60" s="7"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C61" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hourly output : add ID
</commit_message>
<xml_diff>
--- a/inst/application/www/Output_Selection_template.xlsx
+++ b/inst/application/www/Output_Selection_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BenoitThieurmel\Documents\git\antaresVizMedTSO\inst\application\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CF43FE-6DAD-4BB2-8B44-FEF801B5BB54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E890ECD-0727-4A05-A9C3-3D1E5ED8B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D77C83E6-B695-4B37-B3DE-F053925C20A4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D77C83E6-B695-4B37-B3DE-F053925C20A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Annual_Selection" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="290">
   <si>
     <t>Links</t>
   </si>
@@ -894,6 +894,15 @@
   </si>
   <si>
     <t>ifelse(`PSP` &lt; 0, as.numeric(`PSP`), 0)</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>TURB</t>
+  </si>
+  <si>
+    <t>PUMP</t>
   </si>
 </sst>
 </file>
@@ -2332,7 +2341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA0C1F2-E3A3-48EB-881E-BF01D90AA1B6}">
   <dimension ref="A1:D119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -3221,10 +3230,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B57E84-B55D-4563-ABB5-693AD42469D5}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3232,9 +3241,10 @@
     <col min="1" max="1" width="26.6640625" style="21" customWidth="1"/>
     <col min="2" max="2" width="37.109375" style="21" customWidth="1"/>
     <col min="3" max="3" width="68.5546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>222</v>
       </c>
@@ -3244,8 +3254,11 @@
       <c r="C1" s="13" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="11" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>162</v>
       </c>
@@ -3255,8 +3268,11 @@
       <c r="C2" s="15" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>163</v>
       </c>
@@ -3266,8 +3282,11 @@
       <c r="C3" s="15" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D3" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>164</v>
       </c>
@@ -3277,8 +3296,11 @@
       <c r="C4" s="15" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>165</v>
       </c>
@@ -3288,8 +3310,11 @@
       <c r="C5" s="15" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>166</v>
       </c>
@@ -3299,8 +3324,11 @@
       <c r="C6" s="15" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>167</v>
       </c>
@@ -3310,8 +3338,11 @@
       <c r="C7" s="15" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>168</v>
       </c>
@@ -3321,8 +3352,11 @@
       <c r="C8" s="15" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>169</v>
       </c>
@@ -3332,8 +3366,11 @@
       <c r="C9" s="15" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>170</v>
       </c>
@@ -3343,8 +3380,11 @@
       <c r="C10" s="15" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>171</v>
       </c>
@@ -3354,8 +3394,11 @@
       <c r="C11" s="15" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="16" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>172</v>
       </c>
@@ -3365,8 +3408,11 @@
       <c r="C12" s="15" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>173</v>
       </c>
@@ -3376,8 +3422,11 @@
       <c r="C13" s="15" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>174</v>
       </c>
@@ -3387,8 +3436,11 @@
       <c r="C14" s="15" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>175</v>
       </c>
@@ -3398,8 +3450,11 @@
       <c r="C15" s="15" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>176</v>
       </c>
@@ -3409,8 +3464,11 @@
       <c r="C16" s="15" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>177</v>
       </c>
@@ -3420,8 +3478,11 @@
       <c r="C17" s="15" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="16" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>178</v>
       </c>
@@ -3431,8 +3492,11 @@
       <c r="C18" s="15" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>179</v>
       </c>
@@ -3442,8 +3506,11 @@
       <c r="C19" s="15" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>180</v>
       </c>
@@ -3453,8 +3520,11 @@
       <c r="C20" s="15" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>181</v>
       </c>
@@ -3464,8 +3534,11 @@
       <c r="C21" s="15" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>182</v>
       </c>
@@ -3475,8 +3548,11 @@
       <c r="C22" s="15" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="18" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>183</v>
       </c>
@@ -3486,8 +3562,11 @@
       <c r="C23" s="15" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
         <v>184</v>
       </c>
@@ -3497,8 +3576,11 @@
       <c r="C24" s="15" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>185</v>
       </c>
@@ -3508,8 +3590,11 @@
       <c r="C25" s="15" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>186</v>
       </c>
@@ -3519,8 +3604,11 @@
       <c r="C26" s="19" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>187</v>
       </c>
@@ -3530,8 +3618,11 @@
       <c r="C27" s="15" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="16" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>188</v>
       </c>
@@ -3541,8 +3632,11 @@
       <c r="C28" s="15" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="16" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>189</v>
       </c>
@@ -3552,8 +3646,11 @@
       <c r="C29" s="15" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>190</v>
       </c>
@@ -3563,8 +3660,11 @@
       <c r="C30" s="15" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="18" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>191</v>
       </c>
@@ -3574,8 +3674,11 @@
       <c r="C31" s="15" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
         <v>192</v>
       </c>
@@ -3585,8 +3688,11 @@
       <c r="C32" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>193</v>
       </c>
@@ -3596,8 +3702,11 @@
       <c r="C33" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>194</v>
       </c>
@@ -3607,8 +3716,11 @@
       <c r="C34" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>195</v>
       </c>
@@ -3618,8 +3730,11 @@
       <c r="C35" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>196</v>
       </c>
@@ -3629,8 +3744,11 @@
       <c r="C36" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="15" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>197</v>
       </c>
@@ -3640,8 +3758,11 @@
       <c r="C37" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
         <v>198</v>
       </c>
@@ -3651,8 +3772,11 @@
       <c r="C38" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="15" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>199</v>
       </c>
@@ -3662,8 +3786,11 @@
       <c r="C39" s="20" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="16" t="s">
         <v>200</v>
       </c>
@@ -3673,8 +3800,11 @@
       <c r="C40" s="20" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
         <v>201</v>
       </c>
@@ -3684,8 +3814,11 @@
       <c r="C41" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>202</v>
       </c>
@@ -3695,8 +3828,11 @@
       <c r="C42" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>203</v>
       </c>
@@ -3706,8 +3842,11 @@
       <c r="C43" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>204</v>
       </c>
@@ -3717,8 +3856,11 @@
       <c r="C44" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D44" s="15" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>205</v>
       </c>
@@ -3728,8 +3870,11 @@
       <c r="C45" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="15" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>206</v>
       </c>
@@ -3739,8 +3884,11 @@
       <c r="C46" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D46" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>207</v>
       </c>
@@ -3750,8 +3898,11 @@
       <c r="C47" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>208</v>
       </c>
@@ -3761,8 +3912,11 @@
       <c r="C48" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D48" s="15" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="16" t="s">
         <v>209</v>
       </c>
@@ -3772,8 +3926,11 @@
       <c r="C49" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="15" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="16" t="s">
         <v>210</v>
       </c>
@@ -3783,8 +3940,11 @@
       <c r="C50" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="15" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="18" t="s">
         <v>211</v>
       </c>
@@ -3794,8 +3954,11 @@
       <c r="C51" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D51" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>212</v>
       </c>
@@ -3805,8 +3968,11 @@
       <c r="C52" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D52" s="15" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>213</v>
       </c>
@@ -3816,8 +3982,11 @@
       <c r="C53" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="15" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
         <v>214</v>
       </c>
@@ -3827,8 +3996,11 @@
       <c r="C54" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="19" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>215</v>
       </c>
@@ -3838,8 +4010,11 @@
       <c r="C55" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D55" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>216</v>
       </c>
@@ -3849,8 +4024,11 @@
       <c r="C56" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>217</v>
       </c>
@@ -3860,8 +4038,11 @@
       <c r="C57" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D57" s="15" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="18" t="s">
         <v>218</v>
       </c>
@@ -3871,8 +4052,11 @@
       <c r="C58" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D58" s="15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="16" t="s">
         <v>219</v>
       </c>
@@ -3882,8 +4066,11 @@
       <c r="C59" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D59" s="15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>220</v>
       </c>
@@ -3893,8 +4080,11 @@
       <c r="C60" s="15" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D60" s="15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="15" t="s">
         <v>221</v>
       </c>
@@ -3903,6 +4093,9 @@
       </c>
       <c r="C61" s="15" t="s">
         <v>256</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>